<commit_message>
implement another module for gemini pro
</commit_message>
<xml_diff>
--- a/gg.xlsx
+++ b/gg.xlsx
@@ -461,12 +461,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Integrated Steel Company</t>
+          <t>Integrated Steel Company for Cable Tray System(ISP)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>31088287900003</t>
+          <t>31080000057900003</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>3346.43</t>
+          <t>2398.00</t>
         </is>
       </c>
     </row>
@@ -493,17 +493,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Al-Hawamish Trading Est.</t>
+          <t>Al-Hawamah Trading Est.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>30207091600003</t>
+          <t>3020709160003</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2022-08-07</t>
+          <t>2022/08/07</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">

</xml_diff>